<commit_message>
well we have a start
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/Excel_test.xlsx
+++ b/Manipulating Excels with Code/Excel_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SESA733530\Desktop\Bureau\manipulating_excels\Manipulating Excels with Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEB80426-5A87-43A6-AADF-B39AF785565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24279A66-D76E-4C8E-8046-5687CED8231F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{954FDF21-168F-45AB-B23A-57329EC4B510}"/>
   </bookViews>
@@ -36,15 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">Come </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kill</t>
   </si>
   <si>
     <t>Points</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Come</t>
   </si>
 </sst>
 </file>
@@ -399,23 +402,26 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
       <c r="B2">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added the invited section
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/Excel_test.xlsx
+++ b/Manipulating Excels with Code/Excel_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\Bureau\Code Work\manipulating_excels\Manipulating Excels with Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D7D445-C479-4368-AFD5-11286C935878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A3F70B-38F7-4DB2-9BF6-2386BE3BE359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30015" yWindow="4170" windowWidth="19830" windowHeight="14970" xr2:uid="{954FDF21-168F-45AB-B23A-57329EC4B510}"/>
+    <workbookView xWindow="19320" yWindow="5040" windowWidth="21870" windowHeight="15345" xr2:uid="{954FDF21-168F-45AB-B23A-57329EC4B510}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Points</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Joueur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heure </t>
   </si>
   <si>
     <t>Killer</t>
@@ -405,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1509B223-D6B0-43C2-AA9F-A598451C8D97}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,12 +413,12 @@
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -432,9 +429,6 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>